<commit_message>
Doc structure and overview sample.
</commit_message>
<xml_diff>
--- a/template-utils-core/src/test/resources/templates/integrationtests/conditions/vintage/conditions_eco_v11.xlsx
+++ b/template-utils-core/src/test/resources/templates/integrationtests/conditions/vintage/conditions_eco_v11.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="108" windowWidth="19140" windowHeight="9552"/>
   </bookViews>
@@ -18,10 +18,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Levente</author>
+    <author>Szerző</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -32,7 +32,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Levente:</t>
+          <t>Szerző:</t>
         </r>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,6 +163,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -210,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -525,6 +528,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -537,5 +541,6 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feature docstructure e2e tests (#21)
* Doc structure and overview sample.

* Javadoc fix - ValueSet constructor.
</commit_message>
<xml_diff>
--- a/template-utils-core/src/test/resources/templates/integrationtests/conditions/vintage/conditions_eco_v11.xlsx
+++ b/template-utils-core/src/test/resources/templates/integrationtests/conditions/vintage/conditions_eco_v11.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="96" yWindow="108" windowWidth="19140" windowHeight="9552"/>
   </bookViews>
@@ -18,10 +18,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Levente</author>
+    <author>Szerző</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -32,7 +32,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Levente:</t>
+          <t>Szerző:</t>
         </r>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,6 +163,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -210,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -525,6 +528,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -537,5 +541,6 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>